<commit_message>
A wrong index in a constraint has been fixed
</commit_message>
<xml_diff>
--- a/Parte2/mathematicalProgramming/mathematicalProgramming.xlsx
+++ b/Parte2/mathematicalProgramming/mathematicalProgramming.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miren\Desktop\Unige\Methods and Tools for Industrial Automation\Methods\Parte2\mathematicalProgramming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/274eccc78034c9a0/Documenti/MATLAB/Progetto/Methods/Parte2/mathematicalProgramming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA75458-F58D-4B53-B173-B82C1E59A3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{EEA75458-F58D-4B53-B173-B82C1E59A3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCD61301-B7C7-4410-9849-3DE0E363D25A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5AF9F7C8-C9F4-49DE-B92B-8A6DDB58D3EA}"/>
   </bookViews>
@@ -22,40 +22,40 @@
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Foglio1!$I$11</definedName>
-    <definedName name="solver_lhs10" localSheetId="0" hidden="1">Foglio1!$F$19</definedName>
-    <definedName name="solver_lhs11" localSheetId="0" hidden="1">Foglio1!$G$19</definedName>
-    <definedName name="solver_lhs12" localSheetId="0" hidden="1">Foglio1!$F$9</definedName>
-    <definedName name="solver_lhs13" localSheetId="0" hidden="1">Foglio1!$I$19</definedName>
-    <definedName name="solver_lhs14" localSheetId="0" hidden="1">Foglio1!$I$13</definedName>
-    <definedName name="solver_lhs15" localSheetId="0" hidden="1">Foglio1!$H$12</definedName>
-    <definedName name="solver_lhs16" localSheetId="0" hidden="1">Foglio1!$H$19</definedName>
-    <definedName name="solver_lhs17" localSheetId="0" hidden="1">Foglio1!$H$19</definedName>
-    <definedName name="solver_lhs18" localSheetId="0" hidden="1">Foglio1!$I$10</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Foglio1!$E$11</definedName>
+    <definedName name="solver_lhs10" localSheetId="0" hidden="1">Foglio1!$H$19</definedName>
+    <definedName name="solver_lhs11" localSheetId="0" hidden="1">Foglio1!$I$19</definedName>
+    <definedName name="solver_lhs12" localSheetId="0" hidden="1">Foglio1!$I$12</definedName>
+    <definedName name="solver_lhs13" localSheetId="0" hidden="1">Foglio1!$H$19</definedName>
+    <definedName name="solver_lhs14" localSheetId="0" hidden="1">Foglio1!$I$10</definedName>
+    <definedName name="solver_lhs15" localSheetId="0" hidden="1">Foglio1!$G$19</definedName>
+    <definedName name="solver_lhs16" localSheetId="0" hidden="1">Foglio1!$G$19</definedName>
+    <definedName name="solver_lhs17" localSheetId="0" hidden="1">Foglio1!$F$19</definedName>
+    <definedName name="solver_lhs18" localSheetId="0" hidden="1">Foglio1!$G$19</definedName>
     <definedName name="solver_lhs19" localSheetId="0" hidden="1">Foglio1!$H$19</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Foglio1!$E$11</definedName>
-    <definedName name="solver_lhs20" localSheetId="0" hidden="1">Foglio1!$I$12</definedName>
-    <definedName name="solver_lhs21" localSheetId="0" hidden="1">Foglio1!$G$11</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Foglio1!$E$19</definedName>
+    <definedName name="solver_lhs20" localSheetId="0" hidden="1">Foglio1!$I$19</definedName>
+    <definedName name="solver_lhs21" localSheetId="0" hidden="1">Foglio1!$F$9</definedName>
     <definedName name="solver_lhs22" localSheetId="0" hidden="1">Foglio1!$I$19</definedName>
-    <definedName name="solver_lhs23" localSheetId="0" hidden="1">Foglio1!$I$19</definedName>
-    <definedName name="solver_lhs24" localSheetId="0" hidden="1">Foglio1!$G$10</definedName>
-    <definedName name="solver_lhs25" localSheetId="0" hidden="1">Foglio1!$G$19</definedName>
-    <definedName name="solver_lhs26" localSheetId="0" hidden="1">Foglio1!$F$19</definedName>
-    <definedName name="solver_lhs27" localSheetId="0" hidden="1">Foglio1!$I$12</definedName>
-    <definedName name="solver_lhs28" localSheetId="0" hidden="1">Foglio1!$E$9:$I$13</definedName>
-    <definedName name="solver_lhs29" localSheetId="0" hidden="1">Foglio1!$F$19</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Foglio1!$G$19</definedName>
-    <definedName name="solver_lhs30" localSheetId="0" hidden="1">Foglio1!$F$19</definedName>
-    <definedName name="solver_lhs31" localSheetId="0" hidden="1">Foglio1!$F$10</definedName>
-    <definedName name="solver_lhs32" localSheetId="0" hidden="1">Foglio1!$E$19</definedName>
-    <definedName name="solver_lhs33" localSheetId="0" hidden="1">Foglio1!$E$19</definedName>
-    <definedName name="solver_lhs34" localSheetId="0" hidden="1">Foglio1!$E$19</definedName>
-    <definedName name="solver_lhs35" localSheetId="0" hidden="1">Foglio1!$E$9</definedName>
+    <definedName name="solver_lhs23" localSheetId="0" hidden="1">Foglio1!$I$13</definedName>
+    <definedName name="solver_lhs24" localSheetId="0" hidden="1">Foglio1!$H$12</definedName>
+    <definedName name="solver_lhs25" localSheetId="0" hidden="1">Foglio1!$G$11</definedName>
+    <definedName name="solver_lhs26" localSheetId="0" hidden="1">Foglio1!$I$11</definedName>
+    <definedName name="solver_lhs27" localSheetId="0" hidden="1">Foglio1!$G$10</definedName>
+    <definedName name="solver_lhs28" localSheetId="0" hidden="1">Foglio1!$F$19</definedName>
+    <definedName name="solver_lhs29" localSheetId="0" hidden="1">Foglio1!$H$10</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Foglio1!$E$9</definedName>
+    <definedName name="solver_lhs30" localSheetId="0" hidden="1">Foglio1!$H$19</definedName>
+    <definedName name="solver_lhs31" localSheetId="0" hidden="1">Foglio1!$F$19</definedName>
+    <definedName name="solver_lhs32" localSheetId="0" hidden="1">Foglio1!$I$12</definedName>
+    <definedName name="solver_lhs33" localSheetId="0" hidden="1">Foglio1!$E$9:$I$13</definedName>
+    <definedName name="solver_lhs34" localSheetId="0" hidden="1">Foglio1!$F$19</definedName>
+    <definedName name="solver_lhs35" localSheetId="0" hidden="1">Foglio1!$E$19</definedName>
     <definedName name="solver_lhs36" localSheetId="0" hidden="1">Foglio1!$E$10</definedName>
     <definedName name="solver_lhs37" localSheetId="0" hidden="1">Foglio1!$E$13</definedName>
     <definedName name="solver_lhs38" localSheetId="0" hidden="1">Foglio1!$E$12</definedName>
     <definedName name="solver_lhs39" localSheetId="0" hidden="1">Foglio1!$E$19</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Foglio1!$G$19</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Foglio1!$H$11</definedName>
     <definedName name="solver_lhs40" localSheetId="0" hidden="1">Foglio1!$I$12</definedName>
     <definedName name="solver_lhs41" localSheetId="0" hidden="1">Foglio1!$I$19</definedName>
     <definedName name="solver_lhs42" localSheetId="0" hidden="1">Foglio1!$I$19</definedName>
@@ -70,10 +70,10 @@
     <definedName name="solver_lhs50" localSheetId="0" hidden="1">Foglio1!$I$19</definedName>
     <definedName name="solver_lhs51" localSheetId="0" hidden="1">Foglio1!$I$19</definedName>
     <definedName name="solver_lhs52" localSheetId="0" hidden="1">Foglio1!$I$19</definedName>
-    <definedName name="solver_lhs6" localSheetId="0" hidden="1">Foglio1!$H$11</definedName>
-    <definedName name="solver_lhs7" localSheetId="0" hidden="1">Foglio1!$H$10</definedName>
-    <definedName name="solver_lhs8" localSheetId="0" hidden="1">Foglio1!$H$19</definedName>
-    <definedName name="solver_lhs9" localSheetId="0" hidden="1">Foglio1!$I$19</definedName>
+    <definedName name="solver_lhs6" localSheetId="0" hidden="1">Foglio1!$E$19</definedName>
+    <definedName name="solver_lhs7" localSheetId="0" hidden="1">Foglio1!$I$19</definedName>
+    <definedName name="solver_lhs8" localSheetId="0" hidden="1">Foglio1!$G$19</definedName>
+    <definedName name="solver_lhs9" localSheetId="0" hidden="1">Foglio1!$F$10</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
@@ -91,34 +91,34 @@
     <definedName name="solver_rel12" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel13" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel14" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rel15" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel15" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel16" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel17" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel18" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel18" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel19" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rel20" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel20" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel21" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel22" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel23" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel23" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel24" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rel25" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel26" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel25" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel26" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel27" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rel28" localSheetId="0" hidden="1">5</definedName>
-    <definedName name="solver_rel29" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel28" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel29" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel3" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel30" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel31" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rel32" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel33" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel31" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel32" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel33" localSheetId="0" hidden="1">5</definedName>
     <definedName name="solver_rel34" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel35" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel35" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel36" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel37" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel38" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel39" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel40" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel41" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel42" localSheetId="0" hidden="1">3</definedName>
@@ -133,44 +133,44 @@
     <definedName name="solver_rel50" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel51" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel52" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel6" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rel7" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel6" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel7" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel8" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel9" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">1-Foglio1!$G$13</definedName>
-    <definedName name="solver_rhs10" localSheetId="0" hidden="1">Foglio1!$H$19+Foglio1!$F$3-1000*(1-Foglio1!$F$12)</definedName>
-    <definedName name="solver_rhs11" localSheetId="0" hidden="1">Foglio1!$F$19+Foglio1!$G$3-1000*(1-Foglio1!$G$10)</definedName>
+    <definedName name="solver_rel9" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">1-Foglio1!$G$9</definedName>
+    <definedName name="solver_rhs10" localSheetId="0" hidden="1">Foglio1!$F$19+Foglio1!$H$3-1000*(1-Foglio1!$H$10)</definedName>
+    <definedName name="solver_rhs11" localSheetId="0" hidden="1">Foglio1!$E$19+Foglio1!$I$3-1000*(1-Foglio1!$I$9)</definedName>
     <definedName name="solver_rhs12" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs13" localSheetId="0" hidden="1">Foglio1!$H$19+Foglio1!$I$3-1000*(1-Foglio1!$I$12)</definedName>
-    <definedName name="solver_rhs14" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs15" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs16" localSheetId="0" hidden="1">Foglio1!$F$19+Foglio1!$H$3-1000*(1-Foglio1!$H$10)</definedName>
-    <definedName name="solver_rhs17" localSheetId="0" hidden="1">Foglio1!$E$19+Foglio1!$H$3-1000*(1-Foglio1!$H$9)</definedName>
-    <definedName name="solver_rhs18" localSheetId="0" hidden="1">1-Foglio1!$F$13</definedName>
+    <definedName name="solver_rhs13" localSheetId="0" hidden="1">Foglio1!$E$19+Foglio1!$H$3-1000*(1-Foglio1!$H$9)</definedName>
+    <definedName name="solver_rhs14" localSheetId="0" hidden="1">1-Foglio1!$F$13</definedName>
+    <definedName name="solver_rhs15" localSheetId="0" hidden="1">Foglio1!$E$19+Foglio1!$G$3-1000*(1-Foglio1!$G$9)</definedName>
+    <definedName name="solver_rhs16" localSheetId="0" hidden="1">Foglio1!$F$19+Foglio1!$G$3-1000*(1-Foglio1!$G$10)</definedName>
+    <definedName name="solver_rhs17" localSheetId="0" hidden="1">Foglio1!$H$19+Foglio1!$F$3-1000*(1-Foglio1!$F$12)</definedName>
+    <definedName name="solver_rhs18" localSheetId="0" hidden="1">Foglio1!$H$19+Foglio1!$G$3-1000*(1-Foglio1!$G$12)</definedName>
     <definedName name="solver_rhs19" localSheetId="0" hidden="1">Foglio1!$G$19+Foglio1!$H$3-1000*(1-Foglio1!$H$11)</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">1-Foglio1!$G$9</definedName>
-    <definedName name="solver_rhs20" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs21" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs22" localSheetId="0" hidden="1">Foglio1!$F$19+Foglio1!$I$3-1000*(1-Foglio1!$I$10)</definedName>
-    <definedName name="solver_rhs23" localSheetId="0" hidden="1">Foglio1!$E$19+Foglio1!$I$3-1000*(1-Foglio1!$I$9)</definedName>
-    <definedName name="solver_rhs24" localSheetId="0" hidden="1">1-Foglio1!$F$11</definedName>
-    <definedName name="solver_rhs25" localSheetId="0" hidden="1">Foglio1!$H$19+Foglio1!$G$3-1000*(1-Foglio1!$G$12)</definedName>
-    <definedName name="solver_rhs26" localSheetId="0" hidden="1">Foglio1!$G$19+Foglio1!$F$3-1000*(1-Foglio1!$F$11)</definedName>
-    <definedName name="solver_rhs27" localSheetId="0" hidden="1">1-Foglio1!$H$13</definedName>
-    <definedName name="solver_rhs28" localSheetId="0" hidden="1">"binario"</definedName>
-    <definedName name="solver_rhs29" localSheetId="0" hidden="1">Foglio1!$E$19+Foglio1!$F$3-1000*(1-Foglio1!$F$9)</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Foglio1!$E$19+Foglio1!$G$3-1000*(1-Foglio1!$G$9)</definedName>
-    <definedName name="solver_rhs30" localSheetId="0" hidden="1">Foglio1!$I$19+Foglio1!$F$3-1000*(1-Foglio1!$F$13)</definedName>
-    <definedName name="solver_rhs31" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs32" localSheetId="0" hidden="1">Foglio1!$G$19+Foglio1!$E$3-1000*(1-Foglio1!$E$11)</definedName>
-    <definedName name="solver_rhs33" localSheetId="0" hidden="1">Foglio1!$I$19+Foglio1!$E$3-1000*(1-Foglio1!$E$13)</definedName>
-    <definedName name="solver_rhs34" localSheetId="0" hidden="1">Foglio1!$H$19+Foglio1!$E$3-1000*(1-Foglio1!$E$12)</definedName>
-    <definedName name="solver_rhs35" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">Foglio1!$I$19+Foglio1!$E$3-1000*(1-Foglio1!$E$13)</definedName>
+    <definedName name="solver_rhs20" localSheetId="0" hidden="1">Foglio1!$F$19+Foglio1!$I$3-1000*(1-Foglio1!$I$10)</definedName>
+    <definedName name="solver_rhs21" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs22" localSheetId="0" hidden="1">Foglio1!$H$19+Foglio1!$I$3-1000*(1-Foglio1!$I$12)</definedName>
+    <definedName name="solver_rhs23" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs24" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs25" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs26" localSheetId="0" hidden="1">1-Foglio1!$G$13</definedName>
+    <definedName name="solver_rhs27" localSheetId="0" hidden="1">1-Foglio1!$F$11</definedName>
+    <definedName name="solver_rhs28" localSheetId="0" hidden="1">Foglio1!$G$19+Foglio1!$F$3-1000*(1-Foglio1!$F$11)</definedName>
+    <definedName name="solver_rhs29" localSheetId="0" hidden="1">1-Foglio1!$F$12</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs30" localSheetId="0" hidden="1">Foglio1!$I$19+Foglio1!$H$3-1000*(1-Foglio1!$H$13)</definedName>
+    <definedName name="solver_rhs31" localSheetId="0" hidden="1">Foglio1!$I$19+Foglio1!$F$3-1000*(1-Foglio1!$F$13)</definedName>
+    <definedName name="solver_rhs32" localSheetId="0" hidden="1">1-Foglio1!$H$13</definedName>
+    <definedName name="solver_rhs33" localSheetId="0" hidden="1">"binario"</definedName>
+    <definedName name="solver_rhs34" localSheetId="0" hidden="1">Foglio1!$E$19+Foglio1!$F$3-1000*(1-Foglio1!$F$9)</definedName>
+    <definedName name="solver_rhs35" localSheetId="0" hidden="1">Foglio1!$H$19+Foglio1!$E$3-1000*(1-Foglio1!$E$12)</definedName>
     <definedName name="solver_rhs36" localSheetId="0" hidden="1">1-Foglio1!$F$9</definedName>
     <definedName name="solver_rhs37" localSheetId="0" hidden="1">1-Foglio1!$I$9</definedName>
     <definedName name="solver_rhs38" localSheetId="0" hidden="1">1-Foglio1!$H$9</definedName>
     <definedName name="solver_rhs39" localSheetId="0" hidden="1">Foglio1!$F$19+Foglio1!$E$3-1000*(1-Foglio1!$E$10)</definedName>
-    <definedName name="solver_rhs4" localSheetId="0" hidden="1">Foglio1!$I$19+Foglio1!$G$3-1000*(1-Foglio1!$G$13)</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">1-Foglio1!$G$12</definedName>
     <definedName name="solver_rhs40" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs41" localSheetId="0" hidden="1">Foglio1!$H$19+Foglio1!$I$3-1000*(1-Foglio1!$I$12)</definedName>
     <definedName name="solver_rhs42" localSheetId="0" hidden="1">Foglio1!$H$19+Foglio1!$I$3-1000*(1-Foglio1!$I$12)</definedName>
@@ -185,10 +185,10 @@
     <definedName name="solver_rhs50" localSheetId="0" hidden="1">Foglio1!$H$19+Foglio1!$I$3-1000*(1-Foglio1!$I$12)</definedName>
     <definedName name="solver_rhs51" localSheetId="0" hidden="1">Foglio1!$H$19+Foglio1!$I$3-1000*(1-Foglio1!$I$12)</definedName>
     <definedName name="solver_rhs52" localSheetId="0" hidden="1">Foglio1!$H$19+Foglio1!$I$3-1000*(1-Foglio1!$I$12)</definedName>
-    <definedName name="solver_rhs6" localSheetId="0" hidden="1">1-Foglio1!$G$12</definedName>
-    <definedName name="solver_rhs7" localSheetId="0" hidden="1">1-Foglio1!$F$12</definedName>
-    <definedName name="solver_rhs8" localSheetId="0" hidden="1">Foglio1!$I$19+Foglio1!$H$3-1000*(1-Foglio1!$H$13)</definedName>
-    <definedName name="solver_rhs9" localSheetId="0" hidden="1">Foglio1!$G$19+Foglio1!$I$3-1000*(1-Foglio1!$I$11)</definedName>
+    <definedName name="solver_rhs6" localSheetId="0" hidden="1">Foglio1!$G$19+Foglio1!$E$3-1000*(1-Foglio1!$E$11)</definedName>
+    <definedName name="solver_rhs7" localSheetId="0" hidden="1">Foglio1!$G$19+Foglio1!$I$3-1000*(1-Foglio1!$I$11)</definedName>
+    <definedName name="solver_rhs8" localSheetId="0" hidden="1">Foglio1!$I$19+Foglio1!$G$3-1000*(1-Foglio1!$G$13)</definedName>
+    <definedName name="solver_rhs9" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
@@ -200,19 +200,10 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -485,6 +476,94 @@
     </r>
   </si>
   <si>
+    <t>Minimize total weighted tardiness</t>
+  </si>
+  <si>
+    <r>
+      <t>Σ w</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">i </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <t>∀ i, j with i ≠ j</t>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ij</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ji</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 1                </t>
+    </r>
+  </si>
+  <si>
+    <t>Optimal sequence</t>
+  </si>
+  <si>
     <r>
       <t>C</t>
     </r>
@@ -539,7 +618,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>i</t>
+      <t>j</t>
     </r>
     <r>
       <rPr>
@@ -572,94 +651,6 @@
       </rPr>
       <t xml:space="preserve">) </t>
     </r>
-  </si>
-  <si>
-    <t>Minimize total weighted tardiness</t>
-  </si>
-  <si>
-    <r>
-      <t>Σ w</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">i </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>i</t>
-    </r>
-  </si>
-  <si>
-    <t>∀ i, j with i ≠ j</t>
-  </si>
-  <si>
-    <r>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ij</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> + x</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ji</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = 1                </t>
-    </r>
-  </si>
-  <si>
-    <t>Optimal sequence</t>
   </si>
 </sst>
 </file>
@@ -1109,8 +1100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C7164C1-8EB4-4D5E-85AB-E939FB995734}">
   <dimension ref="B2:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1414,7 +1405,7 @@
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E19" s="1">
         <f>E16+E3</f>
@@ -1439,7 +1430,7 @@
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -1469,10 +1460,10 @@
     </row>
     <row r="23" spans="2:12" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B23" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" s="1">
         <f>MAX(E19-E4,0)</f>
@@ -1497,10 +1488,10 @@
     </row>
     <row r="24" spans="2:12" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1550,7 +1541,7 @@
         <v>29</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L27" s="6"/>
     </row>

</xml_diff>